<commit_message>
this is my progress so far
</commit_message>
<xml_diff>
--- a/cafe94/src/main/java/login/Data.xlsx
+++ b/cafe94/src/main/java/login/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\Projects\Cafe94\cafe94\src\main\java\login\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ceph\IdeaProjects\Cafe94\cafe94\src\main\java\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D147F7-B7BA-4540-9B16-B083CC6C3D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860758C3-9D54-4329-9CA8-B59907B2BA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>FirstName</t>
   </si>
@@ -283,13 +283,24 @@
   </si>
   <si>
     <t>dadasdad</t>
+  </si>
+  <si>
+    <t>CafeMate0005</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CafeMate0006</t>
+  </si>
+  <si>
+    <t>cephard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -345,9 +356,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -385,7 +396,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -491,7 +502,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -633,7 +644,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -641,136 +652,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.5546875"/>
-    <col min="2" max="2" customWidth="true" width="17.33203125"/>
-    <col min="3" max="3" customWidth="true" width="15.0"/>
-    <col min="4" max="4" customWidth="true" width="18.0"/>
-    <col min="5" max="5" customWidth="true" width="22.6640625"/>
-    <col min="6" max="6" customWidth="true" width="11.88671875"/>
-    <col min="7" max="7" customWidth="true" width="10.109375"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s" s="0">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>74</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>76</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>77</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>78</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>78</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>79</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>80</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>81</v>
       </c>
-      <c r="G5" t="s" s="0">
+      <c r="G5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -787,342 +844,342 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.21875"/>
-    <col min="2" max="2" customWidth="true" width="16.5546875"/>
-    <col min="3" max="3" customWidth="true" width="17.21875"/>
-    <col min="4" max="4" customWidth="true" width="12.33203125"/>
-    <col min="5" max="5" customWidth="true" width="12.88671875"/>
-    <col min="6" max="6" customWidth="true" width="9.88671875"/>
-    <col min="7" max="7" customWidth="true" width="12.109375"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="0">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="0">
-        <v>1</v>
-      </c>
-      <c r="C5" s="0">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0">
-        <v>1</v>
-      </c>
-      <c r="G5" s="0">
-        <v>1</v>
-      </c>
-      <c r="H5" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>48</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s" s="0">
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="0">
-        <v>1</v>
-      </c>
-      <c r="C7" s="0">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>55</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="0">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0">
-        <v>1</v>
-      </c>
-      <c r="D9" s="0">
-        <v>1</v>
-      </c>
-      <c r="E9" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="0">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s" s="0">
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="0">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0">
-        <v>1</v>
-      </c>
-      <c r="D13" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s" s="0">
+      <c r="C14" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="0">
-        <v>1</v>
-      </c>
-      <c r="C15" s="0">
-        <v>1</v>
-      </c>
-      <c r="D15" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s" s="0">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="0">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" t="s" s="0">
+      <c r="C18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" s="0">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" s="0">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" s="0">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>1</v>
       </c>
     </row>

</xml_diff>